<commit_message>
Added formatted alcohol report data, removed json
</commit_message>
<xml_diff>
--- a/Formatted-Data/issued_student_degrees.xlsx
+++ b/Formatted-Data/issued_student_degrees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\Formatted-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6292A23-BF1E-4616-8007-94B47DB494CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A003E7-834C-498C-8DD0-21E084A1A709}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregated Degree Data" sheetId="1" r:id="rId1"/>

</xml_diff>